<commit_message>
new GNG latency code (works for both L/R)
</commit_message>
<xml_diff>
--- a/operantanalysis/scripts/output.xlsx
+++ b/operantanalysis/scripts/output.xlsx
@@ -440,16 +440,16 @@
         <v>23</v>
       </c>
       <c r="G2" t="n">
-        <v>38.70967741935484</v>
+        <v>40</v>
       </c>
       <c r="H2" t="n">
-        <v>20.68965517241379</v>
+        <v>23.33333333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1.945</v>
       </c>
       <c r="J2" t="n">
-        <v>2.07</v>
+        <v>2.257</v>
       </c>
       <c r="K2" t="n">
         <v>-11</v>
@@ -477,16 +477,16 @@
         <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>61.29032258064516</v>
+        <v>63.33333333333333</v>
       </c>
       <c r="H3" t="n">
-        <v>86.20689655172413</v>
+        <v>86.66666666666667</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>2.219</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1.798</v>
       </c>
       <c r="K3" t="n">
         <v>15</v>
@@ -514,16 +514,16 @@
         <v>16</v>
       </c>
       <c r="G4" t="n">
-        <v>80.64516129032258</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="H4" t="n">
-        <v>44.82758620689656</v>
+        <v>46.66666666666666</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>2.198</v>
       </c>
       <c r="J4" t="n">
-        <v>2.414</v>
+        <v>2.775</v>
       </c>
       <c r="K4" t="n">
         <v>9</v>
@@ -551,16 +551,16 @@
         <v>5</v>
       </c>
       <c r="G5" t="n">
-        <v>64.51612903225806</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="H5" t="n">
-        <v>82.75862068965517</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2.893</v>
       </c>
       <c r="J5" t="n">
-        <v>2.454</v>
+        <v>2.099</v>
       </c>
       <c r="K5" t="n">
         <v>15</v>
@@ -588,16 +588,16 @@
         <v>11</v>
       </c>
       <c r="G6" t="n">
-        <v>70.96774193548387</v>
+        <v>73.33333333333333</v>
       </c>
       <c r="H6" t="n">
-        <v>62.06896551724138</v>
+        <v>63.33333333333333</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1.553</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>2.352</v>
       </c>
       <c r="K6" t="n">
         <v>11</v>
@@ -625,16 +625,16 @@
         <v>7</v>
       </c>
       <c r="G7" t="n">
-        <v>93.54838709677419</v>
+        <v>96.66666666666667</v>
       </c>
       <c r="H7" t="n">
-        <v>75.86206896551724</v>
+        <v>76.66666666666667</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1.746</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>2.117</v>
       </c>
       <c r="K7" t="n">
         <v>22</v>
@@ -662,16 +662,16 @@
         <v>23</v>
       </c>
       <c r="G8" t="n">
-        <v>48.38709677419355</v>
+        <v>50</v>
       </c>
       <c r="H8" t="n">
-        <v>20.68965517241379</v>
+        <v>23.33333333333333</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>2.679</v>
       </c>
       <c r="J8" t="n">
-        <v>2.779</v>
+        <v>2.967</v>
       </c>
       <c r="K8" t="n">
         <v>-8</v>
@@ -699,16 +699,16 @@
         <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>80.64516129032258</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="H9" t="n">
-        <v>89.65517241379311</v>
+        <v>90</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1.359</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1.623</v>
       </c>
       <c r="K9" t="n">
         <v>22</v>
@@ -736,16 +736,16 @@
         <v>9</v>
       </c>
       <c r="G10" t="n">
-        <v>64.51612903225806</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="H10" t="n">
-        <v>68.96551724137932</v>
+        <v>70</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>2.087</v>
       </c>
       <c r="J10" t="n">
-        <v>2.099</v>
+        <v>2.111</v>
       </c>
       <c r="K10" t="n">
         <v>11</v>
@@ -773,16 +773,16 @@
         <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>90.32258064516128</v>
+        <v>93.33333333333333</v>
       </c>
       <c r="H11" t="n">
-        <v>86.20689655172413</v>
+        <v>86.66666666666667</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>2.186</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>2.251</v>
       </c>
       <c r="K11" t="n">
         <v>24</v>
@@ -810,16 +810,16 @@
         <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>93.54838709677419</v>
+        <v>96.66666666666667</v>
       </c>
       <c r="H12" t="n">
-        <v>89.65517241379311</v>
+        <v>90</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1.963</v>
       </c>
       <c r="J12" t="n">
-        <v>1.888</v>
+        <v>1.806</v>
       </c>
       <c r="K12" t="n">
         <v>26</v>
@@ -847,16 +847,16 @@
         <v>11</v>
       </c>
       <c r="G13" t="n">
-        <v>70.96774193548387</v>
+        <v>73.33333333333333</v>
       </c>
       <c r="H13" t="n">
-        <v>62.06896551724138</v>
+        <v>63.33333333333333</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>2.576</v>
       </c>
       <c r="J13" t="n">
-        <v>2.699</v>
+        <v>2.841</v>
       </c>
       <c r="K13" t="n">
         <v>11</v>
@@ -884,16 +884,16 @@
         <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>93.54838709677419</v>
+        <v>96.66666666666667</v>
       </c>
       <c r="H14" t="n">
-        <v>89.65517241379311</v>
+        <v>90</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1.53</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="K14" t="n">
         <v>26</v>
@@ -921,16 +921,16 @@
         <v>5</v>
       </c>
       <c r="G15" t="n">
-        <v>93.54838709677419</v>
+        <v>96.66666666666667</v>
       </c>
       <c r="H15" t="n">
-        <v>82.75862068965517</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>2.493</v>
       </c>
       <c r="J15" t="n">
-        <v>2.389</v>
+        <v>2.268</v>
       </c>
       <c r="K15" t="n">
         <v>24</v>
@@ -958,16 +958,16 @@
         <v>9</v>
       </c>
       <c r="G16" t="n">
-        <v>87.09677419354838</v>
+        <v>90</v>
       </c>
       <c r="H16" t="n">
-        <v>68.96551724137932</v>
+        <v>70</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>2.119</v>
       </c>
       <c r="J16" t="n">
-        <v>2.46</v>
+        <v>2.899</v>
       </c>
       <c r="K16" t="n">
         <v>18</v>
@@ -995,16 +995,16 @@
         <v>11</v>
       </c>
       <c r="G17" t="n">
-        <v>87.09677419354838</v>
+        <v>90</v>
       </c>
       <c r="H17" t="n">
-        <v>62.06896551724138</v>
+        <v>63.33333333333333</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>2.44</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>2.802</v>
       </c>
       <c r="K17" t="n">
         <v>16</v>
@@ -1032,16 +1032,16 @@
         <v>8</v>
       </c>
       <c r="G18" t="n">
-        <v>83.87096774193549</v>
+        <v>86.66666666666667</v>
       </c>
       <c r="H18" t="n">
-        <v>72.41379310344827</v>
+        <v>73.33333333333333</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1.206</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>1.344</v>
       </c>
       <c r="K18" t="n">
         <v>18</v>
@@ -1069,16 +1069,16 @@
         <v>10</v>
       </c>
       <c r="G19" t="n">
-        <v>67.74193548387096</v>
+        <v>70</v>
       </c>
       <c r="H19" t="n">
-        <v>65.51724137931035</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>3.029</v>
       </c>
       <c r="J19" t="n">
-        <v>3.24</v>
+        <v>3.461</v>
       </c>
       <c r="K19" t="n">
         <v>11</v>
@@ -1106,16 +1106,16 @@
         <v>25</v>
       </c>
       <c r="G20" t="n">
-        <v>32.25806451612903</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="H20" t="n">
-        <v>13.79310344827586</v>
+        <v>16.66666666666666</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>3.072</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1.624</v>
       </c>
       <c r="K20" t="n">
         <v>-15</v>
@@ -1143,16 +1143,16 @@
         <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>87.09677419354838</v>
+        <v>90</v>
       </c>
       <c r="H21" t="n">
-        <v>89.65517241379311</v>
+        <v>90</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1.353</v>
       </c>
       <c r="J21" t="n">
-        <v>1.487</v>
+        <v>1.62</v>
       </c>
       <c r="K21" t="n">
         <v>24</v>
@@ -1180,16 +1180,16 @@
         <v>17</v>
       </c>
       <c r="G22" t="n">
-        <v>45.16129032258064</v>
+        <v>46.66666666666666</v>
       </c>
       <c r="H22" t="n">
-        <v>41.37931034482759</v>
+        <v>43.33333333333334</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>2.891</v>
       </c>
       <c r="J22" t="n">
-        <v>2.96</v>
+        <v>3.04</v>
       </c>
       <c r="K22" t="n">
         <v>-3</v>
@@ -1217,16 +1217,16 @@
         <v>5</v>
       </c>
       <c r="G23" t="n">
-        <v>87.09677419354838</v>
+        <v>90</v>
       </c>
       <c r="H23" t="n">
-        <v>82.75862068965517</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1.696</v>
       </c>
       <c r="J23" t="n">
-        <v>1.883</v>
+        <v>2.078</v>
       </c>
       <c r="K23" t="n">
         <v>22</v>
@@ -1254,16 +1254,16 @@
         <v>7</v>
       </c>
       <c r="G24" t="n">
-        <v>67.74193548387096</v>
+        <v>70</v>
       </c>
       <c r="H24" t="n">
-        <v>75.86206896551724</v>
+        <v>76.66666666666667</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>2.211</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>2.28</v>
       </c>
       <c r="K24" t="n">
         <v>14</v>
@@ -1291,16 +1291,16 @@
         <v>5</v>
       </c>
       <c r="G25" t="n">
-        <v>80.64516129032258</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="H25" t="n">
-        <v>82.75862068965517</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>2.176</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>2.37</v>
       </c>
       <c r="K25" t="n">
         <v>20</v>

</xml_diff>